<commit_message>
Added basic domain service and DA projects
</commit_message>
<xml_diff>
--- a/Unit_Test_Frameworks/Microsoft_Fakes/Microsoft_Fakes_Notes.xlsx
+++ b/Unit_Test_Frameworks/Microsoft_Fakes/Microsoft_Fakes_Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\git\all-languages\all-languages\Unit_Test_Frameworks\Microsoft_Fakes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4FFE76-3B0A-4985-B84D-DD527E056FF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8061A5-2FF1-4076-B955-28EEDF741C70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>The process to STUB / SHIM for methods is same as for properties also</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>But preferable method is to go with INTERFACE if possible as it is best practice to work with interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Experience - </t>
+  </si>
+  <si>
+    <t>Any type of method or property can be STUBBED / SHIMMED using MICROSOFT FAKES framework</t>
+  </si>
+  <si>
+    <t>You can STUB/SHIM that method (or) property in which it is defined.   No inheritance concepts observed here.</t>
   </si>
 </sst>
 </file>
@@ -373,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C13"/>
+  <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,6 +439,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
STUBS samples updated with relevant information
</commit_message>
<xml_diff>
--- a/Unit_Test_Frameworks/Microsoft_Fakes/Microsoft_Fakes_Notes.xlsx
+++ b/Unit_Test_Frameworks/Microsoft_Fakes/Microsoft_Fakes_Notes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\git\all-languages\all-languages\Unit_Test_Frameworks\Microsoft_Fakes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\git\all-languages\Unit_Test_Frameworks\Microsoft_Fakes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8061A5-2FF1-4076-B955-28EEDF741C70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A70E1B-9E45-46C6-B7B2-5FC2F7586376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>The process to STUB / SHIM for methods is same as for properties also</t>
   </si>
@@ -58,19 +58,89 @@
   </si>
   <si>
     <t>You can STUB/SHIM that method (or) property in which it is defined.   No inheritance concepts observed here.</t>
+  </si>
+  <si>
+    <t>D:\R\git\all-languages\Unit_Test_Frameworks\Microsoft_Fakes\Choose between stub and shim types.docx</t>
+  </si>
+  <si>
+    <t>Choose between stub and shim types</t>
+  </si>
+  <si>
+    <t>More details in the next point</t>
+  </si>
+  <si>
+    <t>STUBS</t>
+  </si>
+  <si>
+    <t>Better to have stubs for all the classes in your solution because you have control over them and can implement interfaces</t>
+  </si>
+  <si>
+    <t>STUBS only work with interfaces</t>
+  </si>
+  <si>
+    <t>Can provide alternative implementations for the members defined in this interface.</t>
+  </si>
+  <si>
+    <t>SHIMS</t>
+  </si>
+  <si>
+    <t>D:\R\git\all-languages\Unit_Test_Frameworks\Microsoft_Fakes\Samples\Stub_Method_Property\ServicesTests\Images_From_ObjectBrowser</t>
+  </si>
+  <si>
+    <r>
+      <t>external assemblies such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF171717"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>System.dll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF171717"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> typically are not provided with separate interface definitions, so you must use shims instead.</t>
+    </r>
+  </si>
+  <si>
+    <t>If you don't have control over the code in which you can't implement interfaces then its better to go with SHIMS in this cases only.</t>
+  </si>
+  <si>
+    <t>FOR MORE INORMATION REFER THESE PATHS IN GIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF171717"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF171717"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -99,9 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C18"/>
+  <dimension ref="A2:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,17 +516,79 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C29" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sample for Shim included
</commit_message>
<xml_diff>
--- a/Unit_Test_Frameworks/Microsoft_Fakes/Microsoft_Fakes_Notes.xlsx
+++ b/Unit_Test_Frameworks/Microsoft_Fakes/Microsoft_Fakes_Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\git\all-languages\Unit_Test_Frameworks\Microsoft_Fakes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A70E1B-9E45-46C6-B7B2-5FC2F7586376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE8806F-392A-4217-A738-0CB62A3F13B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>The process to STUB / SHIM for methods is same as for properties also</t>
   </si>
@@ -115,6 +115,39 @@
   </si>
   <si>
     <t>FOR MORE INORMATION REFER THESE PATHS IN GIT</t>
+  </si>
+  <si>
+    <t>SCOPE OF SHIMS</t>
+  </si>
+  <si>
+    <t>Defined shims are used only inside the SHIMS context i.e. with in the below USING block</t>
+  </si>
+  <si>
+    <t>using(ShimsContext.Create())</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   }</t>
+  </si>
+  <si>
+    <t>For STUBS, we need interfaces and so we have to inject into the classess</t>
+  </si>
+  <si>
+    <t>WHAT IS THE PURPOSE OF "ShimPatientService"   VS "ShimPatientService.AllInstances"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ShimPatientService.AllInstances: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ShimPatientService:    </t>
+  </si>
+  <si>
+    <t>This is to shim(provide alternative implementation) for the INSTANCE &amp; PRIVATE Methods/Properties</t>
+  </si>
+  <si>
+    <t>This is to shim(provide alternative implementation) for the STATIC Methods/Properties</t>
   </si>
 </sst>
 </file>
@@ -453,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C34"/>
+  <dimension ref="A2:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,34 +590,90 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="C29" s="2" t="s">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="C30" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>